<commit_message>
Updated `merge.py` to streamline the merging process and handle column widths.
</commit_message>
<xml_diff>
--- a/f.xlsx
+++ b/f.xlsx
@@ -516,7 +516,7 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -527,7 +527,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -540,7 +540,7 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -1340,7 +1340,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="139" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A62" sqref="$A1:$XFD62"/>
+      <selection activeCell="A1" sqref="A1:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="4"/>

</xml_diff>